<commit_message>
Added two more sets of integration tests to integration-test-cases-g3.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/integration-test-cases-g3.xlsx
+++ b/Documents/Testing/TestDocuments/integration-test-cases-g3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitl\OneDrive\Documents\CANADA\SENECA\ALL COURSES\SEMESTER 2\SFT221\PROJECT\ms5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntg18\Documents\GitHub\winter25-sft221-nee-3\Documents\Testing\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B58A98-2776-4753-A189-7DF943D5055B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C40424-A52F-4430-AF4A-DD4DE654BFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -367,6 +367,579 @@
   </si>
   <si>
     <t>IT404</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">assignPackage and divert:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tests to see if a truck is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> diverted when a package has a valid address on route of the assigned truck</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>SHIPMENT:
+weight = 100kg
+size = 5.0
+Address = (row 3, col 'K')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">assignPackage and divert:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tests to see if a Shipment is assigned to the most optimal Truck (if available) and diverts when the address is not on route.</t>
+    </r>
+  </si>
+  <si>
+    <t>SHIPMENT:
+weight = 100kg
+size = 5.0
+Address = (row 22, col 'B')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns the index of Truck[] corresponding to the green truck
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>divert:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> does not execute</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns the index of Truck[] corresponding to the yellow truck
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>divert:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prints the path the truck has to divert to deliver the package</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">assignPackage and divert:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tests to see if a Shipment is rejected in the event that there are no available Trucks</t>
+    </r>
+  </si>
+  <si>
+    <t>Truck ={(5000, 250), (5000,250), 
+ (5000, 250) }
+SHIPMENT: weight = 100kg
+size = 5.0
+Address = (row 2, col 'B')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns -1 to signal that no Truck was available.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">divert: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>does not execute.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage and divert:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Tests to see if a Shipment is assigned to the next most optimal Truck (if most is unavailable) and diverts</t>
+    </r>
+  </si>
+  <si>
+    <t>SHIPMENT:
+weight = 100kg
+size = 5.0
+Address = (row 3, col 'M')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns the index of Truck[] corresponding to blue assuming green is unavailable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>divert:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prints the path the blue truck has to divert to deliver the package</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">assignPackage and checkSpace:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tests to see if a Shipment is assigned to an available Truck which is closest to the Shipment address</t>
+    </r>
+  </si>
+  <si>
+    <t>Truck = {(1000, 50, Route:blue)}
+SHIPMENT:
+weight = 100kg
+size = 5.0
+Address = (row 8, col 'K')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkSpace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns true</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+assignPackage:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns the index of Truck[] corresponding to the blue truck
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">assignPackage and checkSpace:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tests to see if a Shipment is assigned to the next Truck closest to the Shipment address if the first is full.</t>
+    </r>
+  </si>
+  <si>
+    <t>Truck={(5000, 250, Route:blue), 
+(0, 0, Route:green)}
+SHIPMENT:
+weight = 100kg
+size = 5.0
+Address = (row 8, col 'K')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkSpace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns false when receiving the blue truck as an argument
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns the index of Truck[] corresponding to the green truck as the next closest.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage and checkSpace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+Tests to see if a Shipment is assigned to the next available Truck when the Shipment address is on the same path as all other trucks </t>
+    </r>
+  </si>
+  <si>
+    <t>Truck={(5000, 250, Route:blue), 
+(0, 0, Route:green)}
+SHIPMENT:
+weight = 100kg
+size = 5.0
+Address = (row 2, col 'B')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage and checkSpace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Tests to see if a Shipment is rejected when all trucks are full</t>
+    </r>
+  </si>
+  <si>
+    <t>Truck={(5000, 250, Route:blue), 
+(5000, 250, Route:green), 
+(5000, 250, Route:yellow)}
+SHIPMENT:
+weight = 100kg
+size = 5.0
+Address = (row 2, col 'B')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkSpace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns false for all trucks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assignPackage:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prints a message stating the package will "Ship tomorrow" and returns -1</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -424,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -436,6 +1009,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,17 +1307,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="5" width="26.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="3" max="5" width="26.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +1337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -763,7 +1351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -777,7 +1365,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -791,7 +1379,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -805,7 +1393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
@@ -813,7 +1401,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -827,7 +1415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -841,7 +1429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -855,7 +1443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -869,7 +1457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="5"/>
@@ -877,27 +1465,71 @@
       <c r="E11" s="5"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="5"/>
@@ -905,25 +1537,69 @@
       <c r="E16" s="5"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="B20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>